<commit_message>
Up and SCRUM added
</commit_message>
<xml_diff>
--- a/Thrash/CourseAssignment/burndownChart.xlsx
+++ b/Thrash/CourseAssignment/burndownChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudiu\Desktop\SEP2\SEP2Group\CourseAssignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudiu\Desktop\SEP2\SEP2Group\Thrash\CourseAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA2A07C-DF32-4EF9-A915-2BFA75A96AB2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF43F909-2E11-4823-A67B-91719C6D76C2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{16860CCE-BD4E-434D-99B6-05202FD211FB}"/>
   </bookViews>
@@ -25,39 +25,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>23/04/2018</t>
+    <t>Sprint 1</t>
   </si>
   <si>
-    <t>24/04/2018</t>
+    <t>Sprint 3</t>
   </si>
   <si>
-    <t>25/04/2018</t>
+    <t>Sprint 2</t>
   </si>
   <si>
-    <t>26/04/2018</t>
+    <t>Sprint 4</t>
   </si>
   <si>
-    <t>27/04/2018</t>
+    <t>Sprint 5</t>
   </si>
   <si>
-    <t>28/04/2018</t>
+    <t xml:space="preserve">20+17+12+7+6 = </t>
   </si>
   <si>
-    <t>29/04/2018</t>
+    <t>Actual Tasks Remaining</t>
   </si>
   <si>
-    <t>30/04/2018</t>
-  </si>
-  <si>
-    <t>Ideal Completion</t>
-  </si>
-  <si>
-    <t>Actual Completion</t>
+    <t>Ideal Tasks Remaining</t>
   </si>
 </sst>
 </file>
@@ -136,8 +130,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10300698867934648"/>
-          <c:y val="2.0904378596129525E-2"/>
+          <c:x val="0.10895049922593618"/>
+          <c:y val="0.10885394340034144"/>
           <c:w val="0.69624907346175924"/>
           <c:h val="0.71229532735374934"/>
         </c:manualLayout>
@@ -154,7 +148,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Actual Completion</c:v>
+                  <c:v>Actual Tasks Remaining</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -179,83 +173,61 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$5:$C$18</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$C$5:$C$18</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$C$5:$C$9</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>23/04/2018</c:v>
+                  <c:v>Sprint 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24/04/2018</c:v>
+                  <c:v>Sprint 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25/04/2018</c:v>
+                  <c:v>Sprint 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26/04/2018</c:v>
+                  <c:v>Sprint 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27/04/2018</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>28/04/2018</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>29/04/2018</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>30/04/2018</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1/5/2018</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2/5/2018</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3/5/2018</c:v>
+                  <c:v>Sprint 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$D$18</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$D$5:$D$18</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$D$5:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -276,7 +248,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ideal Completion</c:v>
+                  <c:v>Ideal Tasks Remaining</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -299,44 +271,58 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>Sprint 1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Sprint 2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Sprint 3</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Sprint 4</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Sprint 5</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$16</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$E$5:$E$16</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$E$5:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -412,7 +398,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Date</a:t>
+                  <a:t>Sprint Number</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1280,16 +1266,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>71435</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1614,10 +1600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E2D784-53F5-4A62-8F14-E71D11A057E2}">
-  <dimension ref="C4:E15"/>
+  <dimension ref="C4:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,137 +1615,111 @@
     <col min="5" max="5" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>62</v>
+      </c>
+      <c r="H5">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>57</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="H6">
+        <v>17</v>
+      </c>
+      <c r="I6">
+        <f>SUM(H5+ H6+ H7+ H8+H9)</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6">
-        <v>8</v>
-      </c>
-      <c r="E6">
-        <v>9</v>
+      <c r="D7">
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <v>38</v>
+      </c>
+      <c r="H7">
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D8">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E8">
+        <v>24</v>
+      </c>
+      <c r="H8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9">
+        <v>12</v>
+      </c>
+      <c r="H9">
         <v>6</v>
       </c>
-      <c r="E9">
-        <v>6</v>
-      </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-      <c r="E10">
-        <v>5</v>
-      </c>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="1">
-        <v>43105</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="1">
-        <v>43136</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="1">
-        <v>43164</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
     </row>
   </sheetData>
   <sortState ref="D5:E14">

</xml_diff>

<commit_message>
Test Cases and Scrump&UP
</commit_message>
<xml_diff>
--- a/Thrash/CourseAssignment/burndownChart.xlsx
+++ b/Thrash/CourseAssignment/burndownChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudiu\Desktop\SEP2\SEP2Group\Thrash\CourseAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF43F909-2E11-4823-A67B-91719C6D76C2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832C72B9-3D7C-4348-82A8-849E73CF1E90}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{16860CCE-BD4E-434D-99B6-05202FD211FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Ideal Tasks Remaining</t>
+  </si>
+  <si>
+    <t>Sprint 6</t>
   </si>
 </sst>
 </file>
@@ -180,9 +183,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet1!$C$5:$C$9</c:f>
+              <c:f>Sheet1!$C$5:$C$10</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Sprint 1</c:v>
                 </c:pt>
@@ -197,6 +200,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Sprint 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -210,24 +216,27 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet1!$D$5:$D$9</c:f>
+              <c:f>Sheet1!$D$5:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>62</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -273,7 +282,7 @@
           </c:marker>
           <c:cat>
             <c:strLit>
-              <c:ptCount val="5"/>
+              <c:ptCount val="6"/>
               <c:pt idx="0">
                 <c:v>Sprint 1</c:v>
               </c:pt>
@@ -288,6 +297,9 @@
               </c:pt>
               <c:pt idx="4">
                 <c:v>Sprint 5</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>Sprint 6</c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -305,24 +317,27 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet1!$E$5:$E$9</c:f>
+              <c:f>Sheet1!$E$5:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>62</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1603,7 +1618,7 @@
   <dimension ref="C4:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,10 +1646,10 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E5">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H5">
         <v>20</v>
@@ -1648,10 +1663,10 @@
         <v>3</v>
       </c>
       <c r="D6">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E6">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H6">
         <v>17</v>
@@ -1666,10 +1681,10 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E7">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="H7">
         <v>12</v>
@@ -1680,10 +1695,10 @@
         <v>4</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E8">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="H8">
         <v>7</v>
@@ -1694,23 +1709,39 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E9">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H9">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
+      <c r="D12">
+        <f>SUM(D5:D11)</f>
+        <v>231</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E5:E11)</f>
+        <v>231</v>
+      </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>

</xml_diff>